<commit_message>
Script rerun upon revision
</commit_message>
<xml_diff>
--- a/Supplementary_tables.xlsx
+++ b/Supplementary_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmatreyek/Library/CloudStorage/GoogleDrive-kmatreyek@gmail.com/My Drive/_Github/SARS2-CoV-2_ACE2_variant_combinations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06F6CB0-784F-7849-A55F-F02C15AEF8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE05F22A-89B1-ED48-88F4-29FA66AC647B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="500" windowWidth="26560" windowHeight="16480" activeTab="4" xr2:uid="{98C70B2F-BD96-EC42-96EB-5C4BACE282B4}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="26560" windowHeight="16480" xr2:uid="{98C70B2F-BD96-EC42-96EB-5C4BACE282B4}"/>
   </bookViews>
   <sheets>
     <sheet name="1_Barcodes" sheetId="4" r:id="rId1"/>
@@ -42,9 +42,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="359">
   <si>
-    <t>Index</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -963,12 +960,6 @@
     <t>G824D_BC</t>
   </si>
   <si>
-    <t>E329G</t>
-  </si>
-  <si>
-    <t>G845A_AttB_[koz-mut]ACE2[E329G]-IRES-mCherry-H2A-P2A-PuroR</t>
-  </si>
-  <si>
     <t>G845A_BC</t>
   </si>
   <si>
@@ -1117,6 +1108,15 @@
   </si>
   <si>
     <t>GTGCCTCGGT</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>G845A_AttB_[koz-mut]ACE2[E329K]-IRES-mCherry-H2A-P2A-PuroR</t>
+  </si>
+  <si>
+    <t>E329K</t>
   </si>
 </sst>
 </file>
@@ -1218,9 +1218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1258,7 +1258,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1364,7 +1364,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1506,7 +1506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1516,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCE14D4-435A-5E42-8262-FDF0469AFD7D}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1527,78 +1527,78 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" t="s">
         <v>216</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>217</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>218</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>219</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>220</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>221</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>222</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>223</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>224</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>225</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>226</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>227</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>228</v>
-      </c>
-      <c r="N1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" t="s">
         <v>230</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>231</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>232</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G2" t="s">
         <v>233</v>
       </c>
-      <c r="F2" t="s">
-        <v>232</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>234</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>235</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>236</v>
-      </c>
-      <c r="J2" t="s">
-        <v>237</v>
       </c>
       <c r="K2" s="6">
         <v>44606</v>
@@ -1607,42 +1607,42 @@
         <v>1446</v>
       </c>
       <c r="M2" t="s">
+        <v>237</v>
+      </c>
+      <c r="N2" t="s">
         <v>238</v>
-      </c>
-      <c r="N2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G3" t="s">
         <v>240</v>
       </c>
-      <c r="D3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F3" t="s">
-        <v>232</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>241</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>235</v>
+      </c>
+      <c r="J3" t="s">
         <v>242</v>
-      </c>
-      <c r="I3" t="s">
-        <v>236</v>
-      </c>
-      <c r="J3" t="s">
-        <v>243</v>
       </c>
       <c r="K3" s="6">
         <v>44606</v>
@@ -1651,42 +1651,42 @@
         <v>1106</v>
       </c>
       <c r="M3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E4" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H4" t="s">
         <v>245</v>
       </c>
-      <c r="F4" t="s">
-        <v>232</v>
-      </c>
-      <c r="G4" t="s">
-        <v>234</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>235</v>
+      </c>
+      <c r="J4" t="s">
         <v>246</v>
-      </c>
-      <c r="I4" t="s">
-        <v>236</v>
-      </c>
-      <c r="J4" t="s">
-        <v>247</v>
       </c>
       <c r="K4" s="6">
         <v>44606</v>
@@ -1695,42 +1695,42 @@
         <v>1433</v>
       </c>
       <c r="M4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" t="s">
         <v>249</v>
       </c>
-      <c r="C5" t="s">
-        <v>240</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F5" t="s">
+        <v>231</v>
+      </c>
+      <c r="G5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H5" t="s">
         <v>250</v>
       </c>
-      <c r="E5" t="s">
-        <v>233</v>
-      </c>
-      <c r="F5" t="s">
-        <v>232</v>
-      </c>
-      <c r="G5" t="s">
-        <v>234</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>235</v>
+      </c>
+      <c r="J5" t="s">
         <v>251</v>
-      </c>
-      <c r="I5" t="s">
-        <v>236</v>
-      </c>
-      <c r="J5" t="s">
-        <v>252</v>
       </c>
       <c r="K5" s="6">
         <v>44606</v>
@@ -1739,42 +1739,42 @@
         <v>441</v>
       </c>
       <c r="M5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" t="s">
+        <v>232</v>
+      </c>
+      <c r="F6" t="s">
+        <v>231</v>
+      </c>
+      <c r="G6" t="s">
+        <v>240</v>
+      </c>
+      <c r="H6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" t="s">
         <v>254</v>
       </c>
-      <c r="C6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D6" t="s">
-        <v>250</v>
-      </c>
-      <c r="E6" t="s">
-        <v>233</v>
-      </c>
-      <c r="F6" t="s">
-        <v>232</v>
-      </c>
-      <c r="G6" t="s">
-        <v>241</v>
-      </c>
-      <c r="H6" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" t="s">
-        <v>255</v>
-      </c>
       <c r="J6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K6" s="6">
         <v>44614</v>
@@ -1786,39 +1786,39 @@
         <v>107</v>
       </c>
       <c r="N6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" t="s">
         <v>240</v>
       </c>
-      <c r="D7" t="s">
-        <v>250</v>
-      </c>
-      <c r="E7" t="s">
-        <v>233</v>
-      </c>
-      <c r="F7" t="s">
-        <v>232</v>
-      </c>
-      <c r="G7" t="s">
-        <v>241</v>
-      </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K7" s="6">
         <v>44614</v>
@@ -1830,39 +1830,39 @@
         <v>208</v>
       </c>
       <c r="N7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F8" t="s">
+        <v>231</v>
+      </c>
+      <c r="G8" t="s">
         <v>240</v>
       </c>
-      <c r="D8" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" t="s">
-        <v>233</v>
-      </c>
-      <c r="F8" t="s">
-        <v>232</v>
-      </c>
-      <c r="G8" t="s">
-        <v>241</v>
-      </c>
       <c r="H8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K8" s="6">
         <v>44614</v>
@@ -1874,39 +1874,39 @@
         <v>28</v>
       </c>
       <c r="N8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" t="s">
+        <v>232</v>
+      </c>
+      <c r="F9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G9" t="s">
         <v>240</v>
       </c>
-      <c r="D9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E9" t="s">
-        <v>233</v>
-      </c>
-      <c r="F9" t="s">
-        <v>232</v>
-      </c>
-      <c r="G9" t="s">
-        <v>241</v>
-      </c>
       <c r="H9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K9" s="6">
         <v>44614</v>
@@ -1918,39 +1918,39 @@
         <v>119</v>
       </c>
       <c r="N9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" t="s">
+        <v>232</v>
+      </c>
+      <c r="F10" t="s">
+        <v>231</v>
+      </c>
+      <c r="G10" t="s">
         <v>240</v>
       </c>
-      <c r="D10" t="s">
-        <v>250</v>
-      </c>
-      <c r="E10" t="s">
-        <v>233</v>
-      </c>
-      <c r="F10" t="s">
-        <v>232</v>
-      </c>
-      <c r="G10" t="s">
-        <v>241</v>
-      </c>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K10" s="6">
         <v>44614</v>
@@ -1962,39 +1962,39 @@
         <v>54</v>
       </c>
       <c r="N10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F11" t="s">
+        <v>231</v>
+      </c>
+      <c r="G11" t="s">
         <v>240</v>
       </c>
-      <c r="D11" t="s">
-        <v>250</v>
-      </c>
-      <c r="E11" t="s">
-        <v>233</v>
-      </c>
-      <c r="F11" t="s">
-        <v>232</v>
-      </c>
-      <c r="G11" t="s">
-        <v>241</v>
-      </c>
       <c r="H11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K11" s="6">
         <v>44614</v>
@@ -2006,39 +2006,39 @@
         <v>28</v>
       </c>
       <c r="N11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" t="s">
+        <v>249</v>
+      </c>
+      <c r="E12" t="s">
+        <v>232</v>
+      </c>
+      <c r="F12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G12" t="s">
         <v>240</v>
       </c>
-      <c r="D12" t="s">
-        <v>250</v>
-      </c>
-      <c r="E12" t="s">
-        <v>233</v>
-      </c>
-      <c r="F12" t="s">
-        <v>232</v>
-      </c>
-      <c r="G12" t="s">
-        <v>241</v>
-      </c>
       <c r="H12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K12" s="6">
         <v>44614</v>
@@ -2050,39 +2050,39 @@
         <v>76</v>
       </c>
       <c r="N12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" t="s">
+        <v>232</v>
+      </c>
+      <c r="F13" t="s">
+        <v>231</v>
+      </c>
+      <c r="G13" t="s">
         <v>240</v>
       </c>
-      <c r="D13" t="s">
-        <v>250</v>
-      </c>
-      <c r="E13" t="s">
-        <v>233</v>
-      </c>
-      <c r="F13" t="s">
-        <v>232</v>
-      </c>
-      <c r="G13" t="s">
-        <v>241</v>
-      </c>
       <c r="H13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K13" s="6">
         <v>44614</v>
@@ -2094,39 +2094,39 @@
         <v>447</v>
       </c>
       <c r="N13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E14" t="s">
+        <v>232</v>
+      </c>
+      <c r="F14" t="s">
+        <v>231</v>
+      </c>
+      <c r="G14" t="s">
         <v>240</v>
       </c>
-      <c r="D14" t="s">
-        <v>250</v>
-      </c>
-      <c r="E14" t="s">
-        <v>233</v>
-      </c>
-      <c r="F14" t="s">
-        <v>232</v>
-      </c>
-      <c r="G14" t="s">
-        <v>241</v>
-      </c>
       <c r="H14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K14" s="6">
         <v>44614</v>
@@ -2138,39 +2138,39 @@
         <v>95</v>
       </c>
       <c r="N14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
+        <v>266</v>
+      </c>
+      <c r="D15" t="s">
+        <v>231</v>
+      </c>
+      <c r="E15" t="s">
+        <v>244</v>
+      </c>
+      <c r="F15" t="s">
+        <v>231</v>
+      </c>
+      <c r="G15" t="s">
+        <v>233</v>
+      </c>
+      <c r="H15" t="s">
         <v>267</v>
       </c>
-      <c r="D15" t="s">
-        <v>232</v>
-      </c>
-      <c r="E15" t="s">
-        <v>245</v>
-      </c>
-      <c r="F15" t="s">
-        <v>232</v>
-      </c>
-      <c r="G15" t="s">
-        <v>234</v>
-      </c>
-      <c r="H15" t="s">
-        <v>268</v>
-      </c>
       <c r="I15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K15" s="6">
         <v>44614</v>
@@ -2182,39 +2182,39 @@
         <v>352</v>
       </c>
       <c r="N15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D16" t="s">
+        <v>231</v>
+      </c>
+      <c r="E16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" t="s">
+        <v>231</v>
+      </c>
+      <c r="G16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H16" t="s">
         <v>270</v>
       </c>
-      <c r="D16" t="s">
-        <v>232</v>
-      </c>
-      <c r="E16" t="s">
-        <v>245</v>
-      </c>
-      <c r="F16" t="s">
-        <v>232</v>
-      </c>
-      <c r="G16" t="s">
-        <v>234</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
+        <v>259</v>
+      </c>
+      <c r="J16" t="s">
         <v>271</v>
-      </c>
-      <c r="I16" t="s">
-        <v>260</v>
-      </c>
-      <c r="J16" t="s">
-        <v>272</v>
       </c>
       <c r="K16" s="6">
         <v>44629</v>
@@ -2223,42 +2223,42 @@
         <v>99.5</v>
       </c>
       <c r="M16" t="s">
+        <v>272</v>
+      </c>
+      <c r="N16" t="s">
         <v>273</v>
-      </c>
-      <c r="N16" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
+        <v>275</v>
+      </c>
+      <c r="D17" t="s">
+        <v>231</v>
+      </c>
+      <c r="E17" t="s">
+        <v>244</v>
+      </c>
+      <c r="F17" t="s">
+        <v>231</v>
+      </c>
+      <c r="G17" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" t="s">
         <v>276</v>
       </c>
-      <c r="D17" t="s">
-        <v>232</v>
-      </c>
-      <c r="E17" t="s">
-        <v>245</v>
-      </c>
-      <c r="F17" t="s">
-        <v>232</v>
-      </c>
-      <c r="G17" t="s">
-        <v>234</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
+        <v>259</v>
+      </c>
+      <c r="J17" t="s">
         <v>277</v>
-      </c>
-      <c r="I17" t="s">
-        <v>260</v>
-      </c>
-      <c r="J17" t="s">
-        <v>278</v>
       </c>
       <c r="K17" s="6">
         <v>44629</v>
@@ -2270,39 +2270,39 @@
         <v>70</v>
       </c>
       <c r="N17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D18" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" t="s">
+        <v>244</v>
+      </c>
+      <c r="F18" t="s">
+        <v>231</v>
+      </c>
+      <c r="G18" t="s">
+        <v>233</v>
+      </c>
+      <c r="H18" t="s">
         <v>280</v>
       </c>
-      <c r="D18" t="s">
-        <v>232</v>
-      </c>
-      <c r="E18" t="s">
-        <v>245</v>
-      </c>
-      <c r="F18" t="s">
-        <v>232</v>
-      </c>
-      <c r="G18" t="s">
-        <v>234</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
+        <v>235</v>
+      </c>
+      <c r="J18" t="s">
         <v>281</v>
-      </c>
-      <c r="I18" t="s">
-        <v>236</v>
-      </c>
-      <c r="J18" t="s">
-        <v>282</v>
       </c>
       <c r="K18" s="6">
         <v>44629</v>
@@ -2311,42 +2311,42 @@
         <v>143</v>
       </c>
       <c r="M18" t="s">
+        <v>282</v>
+      </c>
+      <c r="N18" t="s">
         <v>283</v>
-      </c>
-      <c r="N18" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
+        <v>284</v>
+      </c>
+      <c r="D19" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" t="s">
+        <v>244</v>
+      </c>
+      <c r="F19" t="s">
+        <v>231</v>
+      </c>
+      <c r="G19" t="s">
+        <v>233</v>
+      </c>
+      <c r="H19" t="s">
         <v>285</v>
       </c>
-      <c r="D19" t="s">
-        <v>232</v>
-      </c>
-      <c r="E19" t="s">
-        <v>245</v>
-      </c>
-      <c r="F19" t="s">
-        <v>232</v>
-      </c>
-      <c r="G19" t="s">
-        <v>234</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
+        <v>235</v>
+      </c>
+      <c r="J19" t="s">
         <v>286</v>
-      </c>
-      <c r="I19" t="s">
-        <v>236</v>
-      </c>
-      <c r="J19" t="s">
-        <v>287</v>
       </c>
       <c r="K19" s="6">
         <v>44629</v>
@@ -2355,42 +2355,42 @@
         <v>173</v>
       </c>
       <c r="M19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" t="s">
+        <v>231</v>
+      </c>
+      <c r="E20" t="s">
+        <v>244</v>
+      </c>
+      <c r="F20" t="s">
+        <v>231</v>
+      </c>
+      <c r="G20" t="s">
+        <v>233</v>
+      </c>
+      <c r="H20" t="s">
         <v>289</v>
       </c>
-      <c r="D20" t="s">
-        <v>232</v>
-      </c>
-      <c r="E20" t="s">
-        <v>245</v>
-      </c>
-      <c r="F20" t="s">
-        <v>232</v>
-      </c>
-      <c r="G20" t="s">
-        <v>234</v>
-      </c>
-      <c r="H20" t="s">
-        <v>290</v>
-      </c>
       <c r="I20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K20" s="6">
         <v>44629</v>
@@ -2399,42 +2399,42 @@
         <v>100</v>
       </c>
       <c r="M20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
+        <v>291</v>
+      </c>
+      <c r="D21" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F21" t="s">
+        <v>231</v>
+      </c>
+      <c r="G21" t="s">
+        <v>233</v>
+      </c>
+      <c r="H21" t="s">
         <v>292</v>
       </c>
-      <c r="D21" t="s">
-        <v>232</v>
-      </c>
-      <c r="E21" t="s">
-        <v>245</v>
-      </c>
-      <c r="F21" t="s">
-        <v>232</v>
-      </c>
-      <c r="G21" t="s">
-        <v>234</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
+        <v>254</v>
+      </c>
+      <c r="J21" t="s">
         <v>293</v>
-      </c>
-      <c r="I21" t="s">
-        <v>255</v>
-      </c>
-      <c r="J21" t="s">
-        <v>294</v>
       </c>
       <c r="K21" s="6">
         <v>44629</v>
@@ -2443,42 +2443,42 @@
         <v>167</v>
       </c>
       <c r="M21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
+        <v>295</v>
+      </c>
+      <c r="D22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E22" t="s">
+        <v>244</v>
+      </c>
+      <c r="F22" t="s">
+        <v>231</v>
+      </c>
+      <c r="G22" t="s">
+        <v>233</v>
+      </c>
+      <c r="H22" t="s">
         <v>296</v>
       </c>
-      <c r="D22" t="s">
-        <v>232</v>
-      </c>
-      <c r="E22" t="s">
-        <v>245</v>
-      </c>
-      <c r="F22" t="s">
-        <v>232</v>
-      </c>
-      <c r="G22" t="s">
-        <v>234</v>
-      </c>
-      <c r="H22" t="s">
-        <v>297</v>
-      </c>
       <c r="I22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K22" s="6">
         <v>44629</v>
@@ -2490,39 +2490,39 @@
         <v>335</v>
       </c>
       <c r="N22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
+        <v>298</v>
+      </c>
+      <c r="D23" t="s">
+        <v>231</v>
+      </c>
+      <c r="E23" t="s">
+        <v>244</v>
+      </c>
+      <c r="F23" t="s">
+        <v>231</v>
+      </c>
+      <c r="G23" t="s">
+        <v>233</v>
+      </c>
+      <c r="H23" t="s">
         <v>299</v>
       </c>
-      <c r="D23" t="s">
-        <v>232</v>
-      </c>
-      <c r="E23" t="s">
-        <v>245</v>
-      </c>
-      <c r="F23" t="s">
-        <v>232</v>
-      </c>
-      <c r="G23" t="s">
-        <v>234</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>259</v>
+      </c>
+      <c r="J23" t="s">
         <v>300</v>
-      </c>
-      <c r="I23" t="s">
-        <v>260</v>
-      </c>
-      <c r="J23" t="s">
-        <v>301</v>
       </c>
       <c r="K23" s="6">
         <v>44629</v>
@@ -2531,42 +2531,42 @@
         <v>65</v>
       </c>
       <c r="M23" t="s">
+        <v>301</v>
+      </c>
+      <c r="N23" t="s">
         <v>302</v>
-      </c>
-      <c r="N23" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
+        <v>303</v>
+      </c>
+      <c r="D24" t="s">
+        <v>231</v>
+      </c>
+      <c r="E24" t="s">
+        <v>244</v>
+      </c>
+      <c r="F24" t="s">
+        <v>231</v>
+      </c>
+      <c r="G24" t="s">
+        <v>233</v>
+      </c>
+      <c r="H24" t="s">
         <v>304</v>
       </c>
-      <c r="D24" t="s">
-        <v>232</v>
-      </c>
-      <c r="E24" t="s">
-        <v>245</v>
-      </c>
-      <c r="F24" t="s">
-        <v>232</v>
-      </c>
-      <c r="G24" t="s">
-        <v>234</v>
-      </c>
-      <c r="H24" t="s">
-        <v>305</v>
-      </c>
       <c r="I24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K24" s="6">
         <v>44629</v>
@@ -2575,42 +2575,42 @@
         <v>147</v>
       </c>
       <c r="M24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>307</v>
+        <v>358</v>
       </c>
       <c r="D25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H25" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="I25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K25" s="6">
         <v>44629</v>
@@ -2619,42 +2619,42 @@
         <v>219</v>
       </c>
       <c r="M25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N25" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H26" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J26" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="K26" s="6">
         <v>44629</v>
@@ -2663,42 +2663,42 @@
         <v>233</v>
       </c>
       <c r="M26" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="N26" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" t="s">
+        <v>239</v>
+      </c>
+      <c r="D27" t="s">
+        <v>249</v>
+      </c>
+      <c r="E27" t="s">
+        <v>232</v>
+      </c>
+      <c r="F27" t="s">
+        <v>231</v>
+      </c>
+      <c r="G27" t="s">
+        <v>240</v>
+      </c>
+      <c r="H27" t="s">
         <v>149</v>
       </c>
-      <c r="C27" t="s">
-        <v>240</v>
-      </c>
-      <c r="D27" t="s">
-        <v>250</v>
-      </c>
-      <c r="E27" t="s">
-        <v>233</v>
-      </c>
-      <c r="F27" t="s">
-        <v>232</v>
-      </c>
-      <c r="G27" t="s">
-        <v>241</v>
-      </c>
-      <c r="H27" t="s">
-        <v>150</v>
-      </c>
       <c r="I27" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K27" s="6">
         <v>44739</v>
@@ -2707,42 +2707,42 @@
         <v>127</v>
       </c>
       <c r="M27" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="N27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C28" t="s">
+        <v>239</v>
+      </c>
+      <c r="D28" t="s">
+        <v>249</v>
+      </c>
+      <c r="E28" t="s">
+        <v>232</v>
+      </c>
+      <c r="F28" t="s">
+        <v>231</v>
+      </c>
+      <c r="G28" t="s">
         <v>240</v>
       </c>
-      <c r="D28" t="s">
-        <v>250</v>
-      </c>
-      <c r="E28" t="s">
-        <v>233</v>
-      </c>
-      <c r="F28" t="s">
-        <v>232</v>
-      </c>
-      <c r="G28" t="s">
-        <v>241</v>
-      </c>
       <c r="H28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="I28" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K28" s="6">
         <v>44739</v>
@@ -2751,42 +2751,42 @@
         <v>148</v>
       </c>
       <c r="M28" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="N28" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C29" t="s">
+        <v>239</v>
+      </c>
+      <c r="D29" t="s">
+        <v>249</v>
+      </c>
+      <c r="E29" t="s">
+        <v>232</v>
+      </c>
+      <c r="F29" t="s">
+        <v>231</v>
+      </c>
+      <c r="G29" t="s">
         <v>240</v>
       </c>
-      <c r="D29" t="s">
-        <v>250</v>
-      </c>
-      <c r="E29" t="s">
-        <v>233</v>
-      </c>
-      <c r="F29" t="s">
-        <v>232</v>
-      </c>
-      <c r="G29" t="s">
-        <v>241</v>
-      </c>
       <c r="H29" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="I29" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K29" s="6">
         <v>44739</v>
@@ -2795,42 +2795,42 @@
         <v>267</v>
       </c>
       <c r="M29" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="N29" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" t="s">
+        <v>239</v>
+      </c>
+      <c r="D30" t="s">
+        <v>249</v>
+      </c>
+      <c r="E30" t="s">
+        <v>232</v>
+      </c>
+      <c r="F30" t="s">
+        <v>231</v>
+      </c>
+      <c r="G30" t="s">
         <v>240</v>
       </c>
-      <c r="D30" t="s">
-        <v>250</v>
-      </c>
-      <c r="E30" t="s">
-        <v>233</v>
-      </c>
-      <c r="F30" t="s">
-        <v>232</v>
-      </c>
-      <c r="G30" t="s">
-        <v>241</v>
-      </c>
       <c r="H30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K30" s="6">
         <v>44739</v>
@@ -2839,42 +2839,42 @@
         <v>183</v>
       </c>
       <c r="M30" t="s">
+        <v>319</v>
+      </c>
+      <c r="N30" t="s">
         <v>322</v>
-      </c>
-      <c r="N30" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
+        <v>239</v>
+      </c>
+      <c r="D31" t="s">
+        <v>249</v>
+      </c>
+      <c r="E31" t="s">
+        <v>232</v>
+      </c>
+      <c r="F31" t="s">
+        <v>231</v>
+      </c>
+      <c r="G31" t="s">
         <v>240</v>
       </c>
-      <c r="D31" t="s">
-        <v>250</v>
-      </c>
-      <c r="E31" t="s">
-        <v>233</v>
-      </c>
-      <c r="F31" t="s">
-        <v>232</v>
-      </c>
-      <c r="G31" t="s">
-        <v>241</v>
-      </c>
       <c r="H31" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I31" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K31" s="6">
         <v>44739</v>
@@ -2883,10 +2883,10 @@
         <v>224</v>
       </c>
       <c r="M31" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="N31" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2906,288 +2906,288 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3217,713 +3217,713 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3">
+        <f t="shared" ref="G2:G17" si="0">LEN(F2)</f>
+        <v>805</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="3">
-        <f>LEN(F2)</f>
-        <v>805</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="J2" s="3">
-        <f>LEN(I2)</f>
+        <f t="shared" ref="J2:J18" si="1">LEN(I2)</f>
         <v>815</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3">
+        <f t="shared" si="0"/>
+        <v>804</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="3">
-        <f>LEN(F3)</f>
-        <v>804</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="J3" s="3">
-        <f>LEN(I3)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>805</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="3">
-        <f>LEN(F4)</f>
-        <v>805</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="J4" s="3">
-        <f>LEN(I4)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>805</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="3">
-        <f>LEN(F5)</f>
-        <v>805</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="J5" s="3">
-        <f>LEN(I5)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>805</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="3">
-        <f>LEN(F6)</f>
-        <v>805</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="J6" s="3">
-        <f>LEN(I6)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>805</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="3">
-        <f>LEN(F7)</f>
-        <v>805</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="J7" s="3">
-        <f>LEN(I7)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>805</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G8" s="3">
-        <f>LEN(F8)</f>
-        <v>805</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="J8" s="3">
-        <f>LEN(I8)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>805</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G9" s="3">
-        <f>LEN(F9)</f>
-        <v>805</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="J9" s="3">
-        <f>LEN(I9)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>805</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G10" s="3">
-        <f>LEN(F10)</f>
-        <v>805</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="J10" s="3">
-        <f>LEN(I10)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>804</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G11" s="3">
-        <f>LEN(F11)</f>
-        <v>804</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="I11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J11" s="3">
-        <f>LEN(I11)</f>
+        <f t="shared" si="1"/>
         <v>815</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G12" s="3">
-        <f>LEN(F12)</f>
+        <f t="shared" si="0"/>
         <v>805</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J12" s="3">
-        <f>LEN(I12)</f>
+        <f t="shared" si="1"/>
         <v>805</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="G13" s="3">
-        <f>LEN(F13)</f>
+        <f t="shared" si="0"/>
         <v>805</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J13" s="3">
-        <f>LEN(I13)</f>
+        <f t="shared" si="1"/>
         <v>805</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G14" s="3">
-        <f>LEN(F14)</f>
+        <f t="shared" si="0"/>
         <v>805</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J14" s="3">
-        <f>LEN(I14)</f>
+        <f t="shared" si="1"/>
         <v>805</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G15" s="3">
-        <f>LEN(F15)</f>
+        <f t="shared" si="0"/>
         <v>805</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J15" s="3">
-        <f>LEN(I15)</f>
+        <f t="shared" si="1"/>
         <v>805</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" t="s">
+        <v>197</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>1273</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F16" t="s">
-        <v>198</v>
-      </c>
-      <c r="G16" s="3">
-        <f>LEN(F16)</f>
-        <v>1273</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" t="s">
         <v>195</v>
       </c>
-      <c r="I16" t="s">
-        <v>196</v>
-      </c>
       <c r="J16" s="3">
-        <f>LEN(I16)</f>
+        <f t="shared" si="1"/>
         <v>1267</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17" t="s">
+        <v>201</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="0"/>
+        <v>1270</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" t="s">
-        <v>202</v>
-      </c>
-      <c r="G17" s="3">
-        <f>LEN(F17)</f>
-        <v>1270</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="I17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J17" s="3">
-        <f>LEN(I17)</f>
+        <f t="shared" si="1"/>
         <v>1252</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" ref="G18:G21" si="2">LEN(F18)</f>
+        <v>1273</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="G18" s="3">
-        <f t="shared" ref="G18:G21" si="0">LEN(F18)</f>
-        <v>1273</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="I18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J18" s="3">
-        <f>LEN(I18)</f>
+        <f t="shared" si="1"/>
         <v>1255</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="2"/>
+        <v>1271</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="0"/>
-        <v>1271</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="I19" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" ref="J19:J21" si="1">LEN(I19)</f>
+        <f t="shared" ref="J19:J21" si="3">LEN(I19)</f>
         <v>1253</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="2"/>
+        <v>1273</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G20" s="3">
-        <f t="shared" si="0"/>
-        <v>1273</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="I20" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1255</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F21" t="s">
+        <v>213</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="2"/>
+        <v>1270</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F21" t="s">
-        <v>214</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="0"/>
-        <v>1270</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="I21" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1252</v>
       </c>
     </row>
@@ -3937,7 +3937,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3946,31 +3946,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -3978,16 +3981,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -3995,16 +3998,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -4012,16 +4015,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -4029,16 +4032,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -4046,16 +4049,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -4063,16 +4066,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -4080,16 +4083,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -4097,16 +4100,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -4114,16 +4117,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
@@ -4131,16 +4134,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E12" s="2">
         <v>0</v>
@@ -4148,16 +4151,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
@@ -4165,16 +4168,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
@@ -4182,16 +4185,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -4199,16 +4202,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -4216,16 +4219,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -4233,16 +4236,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -4250,16 +4253,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -4267,16 +4270,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -4284,16 +4287,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -4301,16 +4304,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -4318,16 +4321,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -4335,16 +4338,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -4352,16 +4355,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -4369,16 +4372,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -4386,16 +4389,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -4403,16 +4406,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -4420,16 +4423,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -4437,16 +4440,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -4454,16 +4457,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E31" s="2">
         <v>0</v>
@@ -4471,16 +4474,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -4488,16 +4491,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -4505,16 +4508,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -4522,16 +4525,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -4539,16 +4542,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E36">
         <v>5</v>
@@ -4556,16 +4559,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -4573,16 +4576,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E38">
         <v>6</v>
@@ -4590,16 +4593,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -4607,16 +4610,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E40">
         <v>7</v>
@@ -4624,101 +4627,101 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E42">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E44">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E45">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -4726,110 +4729,113 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E47">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E48">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E50">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E51">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C53" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E52">
+    <sortCondition ref="B2:B52"/>
+  </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4839,7 +4845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB47A21-5A33-7E44-9B0E-C310E9F45F5C}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -4847,244 +4853,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" t="s">
         <v>332</v>
-      </c>
-      <c r="C4" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B6" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B9" t="s">
+        <v>335</v>
+      </c>
+      <c r="C9" t="s">
         <v>338</v>
-      </c>
-      <c r="C9" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C10" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C12" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B13" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C13" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B14" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C14" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B15" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C15" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B16" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C16" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B17" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C17" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B18" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C18" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B19" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C19" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B20" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C20" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B21" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C21" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C22" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>